<commit_message>
Calculate necessary adjustments to samples with poor densities
</commit_message>
<xml_diff>
--- a/data/fractionation/220908 Batch 125 Water_Yr_Summary.xlsx
+++ b/data/fractionation/220908 Batch 125 Water_Yr_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Banfield\WaterYear\SIP\data\fractionation\z_arx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Banfield\WaterYear\SIP\data\fractionation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A534447A-791F-4E03-A1C3-486B85BA635D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FFEBE6-AA1E-4235-9B22-1D61B32068BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-21710" windowWidth="38620" windowHeight="21100" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="22" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="230">
   <si>
     <t>calculated density p(20)</t>
   </si>
@@ -770,9 +770,6 @@
     <t>I</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>Isotope</t>
   </si>
   <si>
@@ -849,12 +846,6 @@
   </si>
   <si>
     <t>1462-conc</t>
-  </si>
-  <si>
-    <t>1461-density</t>
-  </si>
-  <si>
-    <t>1461-conc</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1024,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1166,30 +1157,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thick">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1201,7 +1172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1388,16 +1359,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5157,75 +5123,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AD$4:$AD$25</c:f>
+              <c:f>Summary!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.7161031770000008</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7696484170000026</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7652773770000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7587208170000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7534482500000017</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.745798930000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7392423700000013</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7337785700000019</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7283147700000026</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7217582100000008</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.7162944100000015</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.711021843000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.7046565160000018</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.7011870029999994</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.6937289160000013</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6871723560000014</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.681708556000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.6707809560000015</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.6412764360000018</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.5494845960000028</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.4041475160000019</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.2513523490000011</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6016,132 +5919,17 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AD$5:$AD$23</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1.7696484170000026</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7652773770000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7587208170000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7534482500000017</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.745798930000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7392423700000013</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7337785700000019</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7283147700000026</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7217582100000008</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7162944100000015</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.711021843000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.7046565160000018</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.7011870029999994</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6937289160000013</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.6871723560000014</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.681708556000002</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.6707809560000015</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.6412764360000018</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.5494845960000028</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>Summary!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AE$5:$AE$23</c:f>
+              <c:f>Summary!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-4.1421585674754895E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-4.0198070272982375E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.7717335116147199E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4290614833648733E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.711681642684739E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.13847722810943483</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.4106412780705479</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.86808785614295958</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.8724322425005206</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7122781899369659</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.88159281449787696</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.38866530671083238</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.12164205785267639</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.8640264940433079E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-2.1976704887663677E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-1.7575383004220957E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-3.0040352023525146E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-1.9156683346073445E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-5.8049450634801566E-3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8732,10 +8520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E138FBF1-D534-4F7E-950C-764D2E6B8C19}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -8756,7 +8544,7 @@
         <v>191</v>
       </c>
       <c r="B1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -8764,7 +8552,7 @@
         <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -8784,16 +8572,16 @@
         <v>200</v>
       </c>
       <c r="F4" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="G4" s="27" t="s">
         <v>205</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>206</v>
       </c>
       <c r="H4" s="27" t="s">
         <v>201</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J4" s="27" t="s">
         <v>197</v>
@@ -8829,7 +8617,7 @@
         <v>37</v>
       </c>
       <c r="J5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9072,42 +8860,12 @@
         <v>37</v>
       </c>
       <c r="J13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="65">
-        <f>'Tube Loading'!F39</f>
-        <v>1461</v>
-      </c>
-      <c r="B14" s="65" t="str">
-        <f>'Tube Loading'!A39</f>
-        <v>Tube K</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>202</v>
-      </c>
-      <c r="D14" s="66">
-        <v>44812</v>
-      </c>
-      <c r="E14">
-        <v>135</v>
-      </c>
-      <c r="G14" s="65">
-        <f>'Tube Loading'!J39</f>
-        <v>3000</v>
-      </c>
-      <c r="H14" s="52">
-        <f>Summary!AE26</f>
-        <v>8.4576796737419695</v>
-      </c>
-      <c r="I14" s="67">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>207</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -17365,10 +17123,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA4E3B1-5772-4D1F-AF5A-033072A123CA}">
-  <dimension ref="A1:AE83"/>
+  <dimension ref="A1:AB83"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:AH1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.5"/>
@@ -17383,167 +17141,152 @@
     <col min="12" max="16384" width="10.90625" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="13" thickTop="1">
+    <row r="1" spans="1:28" ht="13" thickTop="1">
       <c r="A1" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="105">
+      <c r="B1" s="102">
         <f>'Tube Loading'!F29</f>
         <v>1547</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="103" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="104" t="s">
         <v>213</v>
       </c>
-      <c r="D1" s="107" t="s">
-        <v>214</v>
-      </c>
-      <c r="E1" s="105">
+      <c r="E1" s="102">
         <f>'Tube Loading'!F30</f>
         <v>1548</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="103" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="104" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="107" t="s">
-        <v>216</v>
-      </c>
-      <c r="H1" s="105">
+      <c r="H1" s="102">
         <f>'Tube Loading'!F31</f>
         <v>1534</v>
       </c>
-      <c r="I1" s="106" t="s">
+      <c r="I1" s="103" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" s="104" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="107" t="s">
-        <v>218</v>
-      </c>
-      <c r="K1" s="105">
+      <c r="K1" s="102">
         <f>'Tube Loading'!F32</f>
         <v>1522</v>
       </c>
-      <c r="L1" s="106" t="s">
+      <c r="L1" s="103" t="s">
+        <v>218</v>
+      </c>
+      <c r="M1" s="104" t="s">
         <v>219</v>
       </c>
-      <c r="M1" s="107" t="s">
-        <v>220</v>
-      </c>
-      <c r="N1" s="104">
+      <c r="N1" s="101">
         <f>'Tube Loading'!F33</f>
         <v>1535</v>
       </c>
-      <c r="O1" s="106" t="s">
+      <c r="O1" s="103" t="s">
+        <v>220</v>
+      </c>
+      <c r="P1" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="P1" s="107" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q1" s="104">
+      <c r="Q1" s="101">
         <f>'Tube Loading'!F34</f>
         <v>1521</v>
       </c>
-      <c r="R1" s="106" t="s">
+      <c r="R1" s="103" t="s">
+        <v>222</v>
+      </c>
+      <c r="S1" s="104" t="s">
         <v>223</v>
       </c>
-      <c r="S1" s="107" t="s">
-        <v>224</v>
-      </c>
-      <c r="T1" s="104">
+      <c r="T1" s="101">
         <f>'Tube Loading'!F35</f>
         <v>1453</v>
       </c>
-      <c r="U1" s="106" t="s">
+      <c r="U1" s="103" t="s">
+        <v>224</v>
+      </c>
+      <c r="V1" s="104" t="s">
         <v>225</v>
       </c>
-      <c r="V1" s="107" t="s">
-        <v>226</v>
-      </c>
-      <c r="W1" s="104">
+      <c r="W1" s="101">
         <f>'Tube Loading'!F36</f>
         <v>1470</v>
       </c>
-      <c r="X1" s="106" t="s">
+      <c r="X1" s="103" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y1" s="104" t="s">
         <v>227</v>
       </c>
-      <c r="Y1" s="107" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z1" s="104">
+      <c r="Z1" s="101">
         <f>'Tube Loading'!F37</f>
         <v>1462</v>
       </c>
-      <c r="AA1" s="106" t="s">
+      <c r="AA1" s="103" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB1" s="104" t="s">
         <v>229</v>
       </c>
-      <c r="AB1" s="107" t="s">
-        <v>230</v>
-      </c>
-      <c r="AC1" s="104">
-        <f>'Tube Loading'!F39</f>
-        <v>1461</v>
-      </c>
-      <c r="AD1" s="106" t="s">
-        <v>231</v>
-      </c>
-      <c r="AE1" s="107" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31">
+    </row>
+    <row r="2" spans="1:28">
       <c r="A2" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="108" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="111" t="s">
+      <c r="C2" s="109"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="112"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="111" t="s">
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="108" t="s">
         <v>171</v>
       </c>
-      <c r="I2" s="112"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="111" t="s">
+      <c r="I2" s="109"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="L2" s="112"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="108" t="s">
+      <c r="L2" s="109"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="105" t="s">
         <v>174</v>
       </c>
-      <c r="O2" s="109"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="108" t="s">
+      <c r="O2" s="106"/>
+      <c r="P2" s="107"/>
+      <c r="Q2" s="105" t="s">
         <v>175</v>
       </c>
-      <c r="R2" s="109"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="108" t="s">
+      <c r="R2" s="106"/>
+      <c r="S2" s="107"/>
+      <c r="T2" s="105" t="s">
         <v>176</v>
       </c>
-      <c r="U2" s="109"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="108" t="s">
+      <c r="U2" s="106"/>
+      <c r="V2" s="107"/>
+      <c r="W2" s="105" t="s">
         <v>177</v>
       </c>
-      <c r="X2" s="109"/>
-      <c r="Y2" s="110"/>
-      <c r="Z2" s="108" t="s">
+      <c r="X2" s="106"/>
+      <c r="Y2" s="107"/>
+      <c r="Z2" s="105" t="s">
         <v>203</v>
       </c>
-      <c r="AA2" s="109"/>
-      <c r="AB2" s="110"/>
-      <c r="AC2" s="108" t="s">
-        <v>204</v>
-      </c>
-      <c r="AD2" s="109"/>
-      <c r="AE2" s="110"/>
-    </row>
-    <row r="3" spans="1:31">
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="107"/>
+    </row>
+    <row r="3" spans="1:28">
       <c r="A3" s="61" t="s">
         <v>168</v>
       </c>
@@ -17628,17 +17371,8 @@
       <c r="AB3" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="AC3" s="84" t="s">
-        <v>188</v>
-      </c>
-      <c r="AD3" s="85" t="s">
-        <v>189</v>
-      </c>
-      <c r="AE3" s="86" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
+    </row>
+    <row r="4" spans="1:28">
       <c r="A4" s="55">
         <v>1</v>
       </c>
@@ -17742,19 +17476,8 @@
       <c r="AB4" s="71">
         <v>-3.1934900793580231E-2</v>
       </c>
-      <c r="AC4" s="69" t="str">
-        <f>'Tube K'!G2</f>
-        <v>D6</v>
-      </c>
-      <c r="AD4" s="70">
-        <f>'Tube K'!F2</f>
-        <v>1.7161031770000008</v>
-      </c>
-      <c r="AE4" s="71">
-        <v>-3.103207448709748E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
+    </row>
+    <row r="5" spans="1:28">
       <c r="A5" s="55">
         <v>2</v>
       </c>
@@ -17858,19 +17581,8 @@
       <c r="AB5" s="74">
         <v>-3.9428125376138788E-2</v>
       </c>
-      <c r="AC5" s="72" t="str">
-        <f>'Tube K'!G3</f>
-        <v>C6</v>
-      </c>
-      <c r="AD5" s="73">
-        <f>'Tube K'!F3</f>
-        <v>1.7696484170000026</v>
-      </c>
-      <c r="AE5" s="74">
-        <v>-4.1421585674754895E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31">
+    </row>
+    <row r="6" spans="1:28">
       <c r="A6" s="55">
         <v>3</v>
       </c>
@@ -17974,19 +17686,8 @@
       <c r="AB6" s="74">
         <v>-2.6174718093239232E-2</v>
       </c>
-      <c r="AC6" s="72" t="str">
-        <f>'Tube K'!G4</f>
-        <v>B6</v>
-      </c>
-      <c r="AD6" s="73">
-        <f>'Tube K'!F4</f>
-        <v>1.7652773770000003</v>
-      </c>
-      <c r="AE6" s="74">
-        <v>-4.0198070272982375E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31">
+    </row>
+    <row r="7" spans="1:28">
       <c r="A7" s="55">
         <v>4</v>
       </c>
@@ -18090,19 +17791,8 @@
       <c r="AB7" s="74">
         <v>-3.4432900074100317E-4</v>
       </c>
-      <c r="AC7" s="72" t="str">
-        <f>'Tube K'!G5</f>
-        <v>A6</v>
-      </c>
-      <c r="AD7" s="73">
-        <f>'Tube K'!F5</f>
-        <v>1.7587208170000004</v>
-      </c>
-      <c r="AE7" s="74">
-        <v>-2.7717335116147199E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31">
+    </row>
+    <row r="8" spans="1:28">
       <c r="A8" s="55">
         <v>5</v>
       </c>
@@ -18206,19 +17896,8 @@
       <c r="AB8" s="74">
         <v>9.2522314864716668E-2</v>
       </c>
-      <c r="AC8" s="72" t="str">
-        <f>'Tube K'!G6</f>
-        <v>A7</v>
-      </c>
-      <c r="AD8" s="73">
-        <f>'Tube K'!F6</f>
-        <v>1.7534482500000017</v>
-      </c>
-      <c r="AE8" s="74">
-        <v>1.4290614833648733E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31">
+    </row>
+    <row r="9" spans="1:28">
       <c r="A9" s="55">
         <v>6</v>
       </c>
@@ -18322,19 +18001,8 @@
       <c r="AB9" s="74">
         <v>0.42510770998273212</v>
       </c>
-      <c r="AC9" s="72" t="str">
-        <f>'Tube K'!G7</f>
-        <v>B7</v>
-      </c>
-      <c r="AD9" s="73">
-        <f>'Tube K'!F7</f>
-        <v>1.745798930000003</v>
-      </c>
-      <c r="AE9" s="74">
-        <v>8.711681642684739E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31">
+    </row>
+    <row r="10" spans="1:28">
       <c r="A10" s="55">
         <v>7</v>
       </c>
@@ -18438,19 +18106,8 @@
       <c r="AB10" s="74">
         <v>0.58400833144405484</v>
       </c>
-      <c r="AC10" s="72" t="str">
-        <f>'Tube K'!G8</f>
-        <v>C7</v>
-      </c>
-      <c r="AD10" s="73">
-        <f>'Tube K'!F8</f>
-        <v>1.7392423700000013</v>
-      </c>
-      <c r="AE10" s="74">
-        <v>0.13847722810943483</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31">
+    </row>
+    <row r="11" spans="1:28">
       <c r="A11" s="55">
         <v>8</v>
       </c>
@@ -18554,19 +18211,8 @@
       <c r="AB11" s="74">
         <v>3.3332784162846316</v>
       </c>
-      <c r="AC11" s="72" t="str">
-        <f>'Tube K'!G9</f>
-        <v>D7</v>
-      </c>
-      <c r="AD11" s="73">
-        <f>'Tube K'!F9</f>
-        <v>1.7337785700000019</v>
-      </c>
-      <c r="AE11" s="74">
-        <v>0.4106412780705479</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31">
+    </row>
+    <row r="12" spans="1:28">
       <c r="A12" s="55">
         <v>9</v>
       </c>
@@ -18659,30 +18305,19 @@
         <f t="shared" si="0"/>
         <v>2.4285758602449894</v>
       </c>
-      <c r="Z12" s="101" t="str">
+      <c r="Z12" s="98" t="str">
         <f>'Tube I'!G10</f>
         <v>H2</v>
       </c>
-      <c r="AA12" s="102">
+      <c r="AA12" s="99">
         <f>'Tube I'!F10</f>
         <v>1.7287791930000012</v>
       </c>
-      <c r="AB12" s="103">
+      <c r="AB12" s="100">
         <v>2.89</v>
       </c>
-      <c r="AC12" s="72" t="str">
-        <f>'Tube K'!G10</f>
-        <v>E7</v>
-      </c>
-      <c r="AD12" s="73">
-        <f>'Tube K'!F10</f>
-        <v>1.7283147700000026</v>
-      </c>
-      <c r="AE12" s="74">
-        <v>0.86808785614295958</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31">
+    </row>
+    <row r="13" spans="1:28">
       <c r="A13" s="55">
         <v>10</v>
       </c>
@@ -18786,19 +18421,8 @@
       <c r="AB13" s="74">
         <v>3.4449553234640775</v>
       </c>
-      <c r="AC13" s="72" t="str">
-        <f>'Tube K'!G11</f>
-        <v>F7</v>
-      </c>
-      <c r="AD13" s="73">
-        <f>'Tube K'!F11</f>
-        <v>1.7217582100000008</v>
-      </c>
-      <c r="AE13" s="74">
-        <v>1.8724322425005206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31">
+    </row>
+    <row r="14" spans="1:28">
       <c r="A14" s="55">
         <v>11</v>
       </c>
@@ -18902,19 +18526,8 @@
       <c r="AB14" s="74">
         <v>1.8461794897700894</v>
       </c>
-      <c r="AC14" s="72" t="str">
-        <f>'Tube K'!G12</f>
-        <v>G7</v>
-      </c>
-      <c r="AD14" s="73">
-        <f>'Tube K'!F12</f>
-        <v>1.7162944100000015</v>
-      </c>
-      <c r="AE14" s="74">
-        <v>1.7122781899369659</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31">
+    </row>
+    <row r="15" spans="1:28">
       <c r="A15" s="55">
         <v>12</v>
       </c>
@@ -19018,19 +18631,8 @@
       <c r="AB15" s="74">
         <v>1.5200559941463556</v>
       </c>
-      <c r="AC15" s="72" t="str">
-        <f>'Tube K'!G13</f>
-        <v>H7</v>
-      </c>
-      <c r="AD15" s="73">
-        <f>'Tube K'!F13</f>
-        <v>1.711021843000001</v>
-      </c>
-      <c r="AE15" s="74">
-        <v>0.88159281449787696</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31">
+    </row>
+    <row r="16" spans="1:28">
       <c r="A16" s="55">
         <v>13</v>
       </c>
@@ -19134,19 +18736,8 @@
       <c r="AB16" s="74">
         <v>0.4745617309986418</v>
       </c>
-      <c r="AC16" s="72" t="str">
-        <f>'Tube K'!G14</f>
-        <v>H8</v>
-      </c>
-      <c r="AD16" s="73">
-        <f>'Tube K'!F14</f>
-        <v>1.7046565160000018</v>
-      </c>
-      <c r="AE16" s="74">
-        <v>0.38866530671083238</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31">
+    </row>
+    <row r="17" spans="1:28">
       <c r="A17" s="55">
         <v>14</v>
       </c>
@@ -19250,19 +18841,8 @@
       <c r="AB17" s="74">
         <v>0.15546014520929394</v>
       </c>
-      <c r="AC17" s="72" t="str">
-        <f>'Tube K'!G15</f>
-        <v>G8</v>
-      </c>
-      <c r="AD17" s="73">
-        <f>'Tube K'!F15</f>
-        <v>1.7011870029999994</v>
-      </c>
-      <c r="AE17" s="74">
-        <v>0.12164205785267639</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31">
+    </row>
+    <row r="18" spans="1:28">
       <c r="A18" s="55">
         <v>15</v>
       </c>
@@ -19366,19 +18946,8 @@
       <c r="AB18" s="74">
         <v>0.33739222248196227</v>
       </c>
-      <c r="AC18" s="72" t="str">
-        <f>'Tube K'!G16</f>
-        <v>F8</v>
-      </c>
-      <c r="AD18" s="73">
-        <f>'Tube K'!F16</f>
-        <v>1.6937289160000013</v>
-      </c>
-      <c r="AE18" s="74">
-        <v>3.8640264940433079E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31">
+    </row>
+    <row r="19" spans="1:28">
       <c r="A19" s="55">
         <v>16</v>
       </c>
@@ -19482,19 +19051,8 @@
       <c r="AB19" s="74">
         <v>0.18375278919983992</v>
       </c>
-      <c r="AC19" s="72" t="str">
-        <f>'Tube K'!G17</f>
-        <v>E8</v>
-      </c>
-      <c r="AD19" s="73">
-        <f>'Tube K'!F17</f>
-        <v>1.6871723560000014</v>
-      </c>
-      <c r="AE19" s="74">
-        <v>-2.1976704887663677E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31">
+    </row>
+    <row r="20" spans="1:28">
       <c r="A20" s="55">
         <v>17</v>
       </c>
@@ -19598,19 +19156,8 @@
       <c r="AB20" s="74">
         <v>6.8306126696438776E-2</v>
       </c>
-      <c r="AC20" s="72" t="str">
-        <f>'Tube K'!G18</f>
-        <v>D8</v>
-      </c>
-      <c r="AD20" s="73">
-        <f>'Tube K'!F18</f>
-        <v>1.681708556000002</v>
-      </c>
-      <c r="AE20" s="74">
-        <v>-1.7575383004220957E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31">
+    </row>
+    <row r="21" spans="1:28">
       <c r="A21" s="55">
         <v>18</v>
       </c>
@@ -19714,19 +19261,8 @@
       <c r="AB21" s="74">
         <v>7.473156941387663E-3</v>
       </c>
-      <c r="AC21" s="72" t="str">
-        <f>'Tube K'!G19</f>
-        <v>C8</v>
-      </c>
-      <c r="AD21" s="73">
-        <f>'Tube K'!F19</f>
-        <v>1.6707809560000015</v>
-      </c>
-      <c r="AE21" s="74">
-        <v>-3.0040352023525146E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31">
+    </row>
+    <row r="22" spans="1:28">
       <c r="A22" s="55">
         <v>19</v>
       </c>
@@ -19830,19 +19366,8 @@
       <c r="AB22" s="74">
         <v>-1.3347969436590681E-2</v>
       </c>
-      <c r="AC22" s="72" t="str">
-        <f>'Tube K'!G20</f>
-        <v>B8</v>
-      </c>
-      <c r="AD22" s="73">
-        <f>'Tube K'!F20</f>
-        <v>1.6412764360000018</v>
-      </c>
-      <c r="AE22" s="74">
-        <v>-1.9156683346073445E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31">
+    </row>
+    <row r="23" spans="1:28">
       <c r="A23" s="55">
         <v>20</v>
       </c>
@@ -19946,19 +19471,8 @@
       <c r="AB23" s="74">
         <v>-1.5319051895843877E-2</v>
       </c>
-      <c r="AC23" s="72" t="str">
-        <f>'Tube K'!G21</f>
-        <v>A8</v>
-      </c>
-      <c r="AD23" s="73">
-        <f>'Tube K'!F21</f>
-        <v>1.5494845960000028</v>
-      </c>
-      <c r="AE23" s="74">
-        <v>-5.8049450634801566E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31">
+    </row>
+    <row r="24" spans="1:28">
       <c r="A24" s="55">
         <v>21</v>
       </c>
@@ -20062,19 +19576,8 @@
       <c r="AB24" s="71">
         <v>-6.4185984799308114E-3</v>
       </c>
-      <c r="AC24" s="69" t="str">
-        <f>'Tube K'!G22</f>
-        <v>A9</v>
-      </c>
-      <c r="AD24" s="70">
-        <f>'Tube K'!F22</f>
-        <v>1.4041475160000019</v>
-      </c>
-      <c r="AE24" s="71">
-        <v>1.438577740035569E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" ht="13" thickBot="1">
+    </row>
+    <row r="25" spans="1:28" ht="13" thickBot="1">
       <c r="A25" s="55">
         <v>22</v>
       </c>
@@ -20178,19 +19681,8 @@
       <c r="AB25" s="88">
         <v>-1.3284647877115144E-3</v>
       </c>
-      <c r="AC25" s="89" t="str">
-        <f>'Tube K'!G23</f>
-        <v>B9</v>
-      </c>
-      <c r="AD25" s="90">
-        <f>'Tube K'!F23</f>
-        <v>1.2513523490000011</v>
-      </c>
-      <c r="AE25" s="71">
-        <v>-2.0878667126671132E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" ht="13" thickTop="1">
+    </row>
+    <row r="26" spans="1:28" ht="13" thickTop="1">
       <c r="B26" s="73"/>
       <c r="C26" s="81" t="s">
         <v>190</v>
@@ -20255,24 +19747,16 @@
         <f>SUM(Y5:Y25)*40/'Tube Loading'!J36*100</f>
         <v>35.634148957788078</v>
       </c>
-      <c r="Z26" s="91"/>
-      <c r="AA26" s="92" t="s">
+      <c r="Z26" s="89"/>
+      <c r="AA26" s="90" t="s">
         <v>190</v>
       </c>
       <c r="AB26" s="82">
         <f>SUM(AB5:AB25)*40/'Tube Loading'!J37*100</f>
         <v>20.347589992552031</v>
       </c>
-      <c r="AC26" s="73"/>
-      <c r="AD26" s="81" t="s">
-        <v>190</v>
-      </c>
-      <c r="AE26" s="93">
-        <f>SUM(AE5:AE25)*40/'Tube Loading'!J39*100</f>
-        <v>8.4576796737419695</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31">
+    </row>
+    <row r="27" spans="1:28">
       <c r="B27" s="73"/>
       <c r="C27" s="73"/>
       <c r="D27" s="73"/>
@@ -20286,7 +19770,7 @@
       <c r="L27" s="73"/>
       <c r="M27" s="73"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:28">
       <c r="B28" s="73"/>
       <c r="C28" s="73"/>
       <c r="D28" s="73"/>
@@ -20300,13 +19784,13 @@
       <c r="L28" s="73"/>
       <c r="M28" s="73"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:28">
       <c r="A29" s="61"/>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:28">
       <c r="A30" s="61"/>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:28">
       <c r="A31" s="61"/>
     </row>
     <row r="55" spans="1:13">
@@ -20361,9 +19845,8 @@
       <c r="M83" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AE2"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
@@ -21107,27 +20590,27 @@
       <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="99">
+      <c r="A24" s="96">
         <v>4.55</v>
       </c>
-      <c r="B24" s="99">
+      <c r="B24" s="96">
         <f t="shared" si="0"/>
         <v>1.0405418073960033</v>
       </c>
-      <c r="C24" s="99">
+      <c r="C24" s="96">
         <f t="shared" si="1"/>
         <v>5.5905418073960034</v>
       </c>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99">
+      <c r="D24" s="96"/>
+      <c r="E24" s="96">
         <f>A24</f>
         <v>4.55</v>
       </c>
-      <c r="F24" s="99">
+      <c r="F24" s="96">
         <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
-      <c r="G24" s="100">
+      <c r="G24" s="97">
         <f>B24-F24</f>
         <v>0.8905418073960033</v>
       </c>
@@ -21254,7 +20737,7 @@
         <f t="shared" ref="E29:E40" si="6">D29*10.9276-13.593</f>
         <v>1.7278230279999995</v>
       </c>
-      <c r="F29" s="95">
+      <c r="F29" s="92">
         <v>1547</v>
       </c>
       <c r="G29">
@@ -21292,7 +20775,7 @@
         <f t="shared" si="6"/>
         <v>1.726730267999999</v>
       </c>
-      <c r="F30" s="95">
+      <c r="F30" s="92">
         <v>1548</v>
       </c>
       <c r="G30">
@@ -21330,7 +20813,7 @@
         <f t="shared" si="6"/>
         <v>1.7280142609999984</v>
       </c>
-      <c r="F31" s="95">
+      <c r="F31" s="92">
         <v>1534</v>
       </c>
       <c r="G31">
@@ -21368,7 +20851,7 @@
         <f t="shared" si="6"/>
         <v>1.7280142609999984</v>
       </c>
-      <c r="F32" s="95">
+      <c r="F32" s="92">
         <v>1522</v>
       </c>
       <c r="G32">
@@ -21406,7 +20889,7 @@
         <f t="shared" si="6"/>
         <v>1.7274951999999999</v>
       </c>
-      <c r="F33" s="95">
+      <c r="F33" s="92">
         <v>1535</v>
       </c>
       <c r="G33">
@@ -21444,7 +20927,7 @@
         <f t="shared" si="6"/>
         <v>1.7280142609999984</v>
       </c>
-      <c r="F34" s="96">
+      <c r="F34" s="93">
         <v>1521</v>
       </c>
       <c r="G34">
@@ -21482,7 +20965,7 @@
         <f t="shared" si="6"/>
         <v>1.7292982539999979</v>
       </c>
-      <c r="F35" s="95">
+      <c r="F35" s="92">
         <v>1453</v>
       </c>
       <c r="G35">
@@ -21520,7 +21003,7 @@
         <f t="shared" si="6"/>
         <v>1.7253096799999987</v>
       </c>
-      <c r="F36" s="95">
+      <c r="F36" s="92">
         <v>1470</v>
       </c>
       <c r="G36">
@@ -21558,7 +21041,7 @@
         <f t="shared" si="6"/>
         <v>1.7274951999999999</v>
       </c>
-      <c r="F37" s="95">
+      <c r="F37" s="92">
         <v>1462</v>
       </c>
       <c r="G37">
@@ -21596,7 +21079,7 @@
         <f t="shared" si="6"/>
         <v>1.7253096799999987</v>
       </c>
-      <c r="F38" s="95">
+      <c r="F38" s="92">
         <v>1454</v>
       </c>
       <c r="G38">
@@ -21634,10 +21117,10 @@
         <f t="shared" si="6"/>
         <v>1.726593673</v>
       </c>
-      <c r="F39" s="95">
+      <c r="F39" s="92">
         <v>1461</v>
       </c>
-      <c r="G39" s="98">
+      <c r="G39" s="95">
         <v>36.32</v>
       </c>
       <c r="H39" s="52">
@@ -21672,7 +21155,7 @@
         <f t="shared" si="6"/>
         <v>1.7276864329999988</v>
       </c>
-      <c r="F40" s="97">
+      <c r="F40" s="94">
         <v>1469</v>
       </c>
       <c r="G40">
@@ -21706,7 +21189,7 @@
         <f t="shared" ref="E41:E44" si="14">D41*10.9276-13.593</f>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F41" s="94"/>
+      <c r="F41" s="91"/>
       <c r="H41" s="52" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -21738,7 +21221,7 @@
         <f t="shared" si="14"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F42" s="94"/>
+      <c r="F42" s="91"/>
       <c r="H42" s="52" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -21770,7 +21253,7 @@
         <f t="shared" si="14"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F43" s="94"/>
+      <c r="F43" s="91"/>
       <c r="H43" s="52" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -21802,7 +21285,7 @@
         <f t="shared" si="14"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F44" s="94"/>
+      <c r="F44" s="91"/>
       <c r="H44" s="52" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -21838,7 +21321,7 @@
         <f>D45*10.9276-13.593</f>
         <v>1.8804542810000004</v>
       </c>
-      <c r="F45" s="94"/>
+      <c r="F45" s="91"/>
       <c r="H45" s="52"/>
       <c r="I45" s="52"/>
       <c r="K45" s="52">

</xml_diff>